<commit_message>
Updated documentation. Added new Integration test written using Protractor.
</commit_message>
<xml_diff>
--- a/app/documentation/Test cases.xlsx
+++ b/app/documentation/Test cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Dev Test assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\test-testers\app\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CDF746B0-2D30-40EC-B4BD-4D5B11D7403E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{33BC4268-7B4C-4EAC-B69B-80D3A0FB9D58}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="4470" xr2:uid="{1EB6EBBC-3C8C-41D0-86E2-0E824122AD8B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="45">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -83,12 +83,6 @@
 Name, Image, Description, Class </t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
-    <t>I don’t see any sort functionality in the app</t>
-  </si>
-  <si>
     <t>/app/bikes.json</t>
   </si>
   <si>
@@ -144,6 +138,94 @@
   </si>
   <si>
     <t>The bike list should only show bikes that whose class includes Race, Comfort.</t>
+  </si>
+  <si>
+    <t>The layout of the screen should be defined by a layout that presents as a grid, but resizes to a list when the screen narrow.
+The following class should be expected on the element that generates the bikelist:
+&lt;div ng-repeat="p in filteredProducts" class="col-sm-4"&gt;</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>7 bikes detected from JSON file. 7 bikes detected from app controller.</t>
+  </si>
+  <si>
+    <t>class name confirmed as col-sm-4</t>
+  </si>
+  <si>
+    <t>The definition of all elements has  been confirmed</t>
+  </si>
+  <si>
+    <t>6 bikes should show</t>
+  </si>
+  <si>
+    <t>4 bikes should show</t>
+  </si>
+  <si>
+    <t>Correct</t>
+  </si>
+  <si>
+    <t>3 bikes should show</t>
+  </si>
+  <si>
+    <t>1 bikes should show</t>
+  </si>
+  <si>
+    <t>1.Open app
+2.Filter By Endurance Race and Comfort
+3.Get products on display
+4.Toggle filter off
+5. Recount products</t>
+  </si>
+  <si>
+    <t>1.Open app
+2.Filter By Endurance and Race
+3.Get products on display
+4.Toggle filter off
+5. Recount products</t>
+  </si>
+  <si>
+    <t>1.Open app
+2.Filter By Comfort
+3.Get products on display
+4.Toggle filter off
+5. Recount products</t>
+  </si>
+  <si>
+    <t>1.Open app
+2.Filter By Race
+3.Get products on display
+4.Toggle filter off
+5. Recount products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Open app
+2.Filter By Endurance  
+3.Get products on display
+4.Toggle filter off
+5. Recount products
+</t>
+  </si>
+  <si>
+    <t>1.Open app
+2.Filter By Enduance and Comfort
+3.Get products on display
+4.Toggle filter off
+5. Recount products</t>
+  </si>
+  <si>
+    <t>1.Open app
+2.Filter By Endurance, Race, Comfort
+3.Refresh page
+4.Get products on display</t>
+  </si>
+  <si>
+    <t>1.Open app
+2.Filter By Race and Comfort
+3.Get products on display
+4.Toggle filter off
+5. Recount products</t>
   </si>
 </sst>
 </file>
@@ -531,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D81E9B-038E-4170-BF14-CB70F6D58F91}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +653,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -582,169 +664,385 @@
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="F2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" ht="51.75" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>